<commit_message>
added config activities and variables for emailaccount
</commit_message>
<xml_diff>
--- a/demoRobot/Documents/Config/config.xlsx
+++ b/demoRobot/Documents/Config/config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dswindle\OneDrive - Capgemini\Documents\DEFRA\UiPath-Templates\Attended Process Template\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953857\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9F8128-AD06-4CC0-AE67-130C5FE388F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -40,12 +39,27 @@
   </si>
   <si>
     <t>Regex</t>
+  </si>
+  <si>
+    <t>boolBreakpoint1</t>
+  </si>
+  <si>
+    <t>breakpoint parameter</t>
+  </si>
+  <si>
+    <t>strEmailAccount</t>
+  </si>
+  <si>
+    <t>azim.karim@defra.gov.uk</t>
+  </si>
+  <si>
+    <t>outlook email account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,12 +179,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -472,11 +485,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,14 +518,36 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Demo Robot with attachment validation
checks attachments for company house header, writes logs file to desktop
</commit_message>
<xml_diff>
--- a/demoRobot/Documents/Config/config.xlsx
+++ b/demoRobot/Documents/Config/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953857\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ADH363FS\x953234$\UiPath\dracoe\demoRobot\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,10 +50,10 @@
     <t>strEmailAccount</t>
   </si>
   <si>
-    <t>azim.karim@defra.gov.uk</t>
-  </si>
-  <si>
     <t>outlook email account</t>
+  </si>
+  <si>
+    <t>Sean.Crotty@defra.gov.uk</t>
   </si>
 </sst>
 </file>
@@ -489,18 +489,18 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B18" sqref="B18:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="4" customWidth="1"/>
     <col min="3" max="3" width="38" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,14 +511,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -529,23 +529,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
     </row>

</xml_diff>

<commit_message>
Demo Robot (Error Messages Corrected)
Final Version worked on by Sean. Error Messages updated.
</commit_message>
<xml_diff>
--- a/demoRobot/Documents/Config/config.xlsx
+++ b/demoRobot/Documents/Config/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ADH363FS\x953234$\UiPath\dracoe\demoRobot\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953234\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t xml:space="preserve"> ROBOT PARAMETERS</t>
+  </si>
+  <si>
+    <t>Regex</t>
+  </si>
+  <si>
+    <t>boolBreakpoint1</t>
+  </si>
+  <si>
+    <t>breakpoint parameter</t>
+  </si>
+  <si>
+    <t>strEmailAccount</t>
+  </si>
+  <si>
+    <t>outlook email account</t>
+  </si>
+  <si>
+    <t>Sean.Crotty@defra.gov.uk</t>
+  </si>
+  <si>
+    <t>LogFilePath</t>
+  </si>
+  <si>
+    <t>log file path</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -35,25 +62,16 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve"> ROBOT PARAMETERS</t>
-  </si>
-  <si>
-    <t>Regex</t>
-  </si>
-  <si>
-    <t>boolBreakpoint1</t>
-  </si>
-  <si>
-    <t>breakpoint parameter</t>
-  </si>
-  <si>
-    <t>strEmailAccount</t>
-  </si>
-  <si>
-    <t>outlook email account</t>
-  </si>
-  <si>
-    <t>Sean.Crotty@defra.gov.uk</t>
+    <t>C:\Users\{0}\Desktop\Demo Robot Log_{1}.xlsx</t>
+  </si>
+  <si>
+    <t>WorkpackageName</t>
+  </si>
+  <si>
+    <t>Demo Robot</t>
+  </si>
+  <si>
+    <t>workpackage name</t>
   </si>
 </sst>
 </file>
@@ -179,7 +197,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <tableColumns count="3">
     <tableColumn id="1" name="Name" dataDxfId="2"/>
     <tableColumn id="2" name="Value" dataDxfId="1"/>
@@ -486,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,31 +520,31 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -534,20 +552,42 @@
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Began working on framework model and using new standards
</commit_message>
<xml_diff>
--- a/demoRobot/Documents/Config/config.xlsx
+++ b/demoRobot/Documents/Config/config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953234\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\dracoe\demoRobot\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC77B70-11D2-47ED-AC5D-33B9F1372F74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t xml:space="preserve"> ROBOT PARAMETERS</t>
   </si>
@@ -72,12 +73,27 @@
   </si>
   <si>
     <t>workpackage name</t>
+  </si>
+  <si>
+    <t>StartPopUpText</t>
+  </si>
+  <si>
+    <t>The popup text to be displayed to the user at the start of the process.</t>
+  </si>
+  <si>
+    <t>StartPopUpTitle</t>
+  </si>
+  <si>
+    <t>Companies House Demo Robot</t>
+  </si>
+  <si>
+    <t>The title of the start pop up.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,11 +213,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C10" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <tableColumns count="3">
-    <tableColumn id="1" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -503,22 +519,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="4" customWidth="1"/>
     <col min="3" max="3" width="38" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="3"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -529,14 +545,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -547,7 +563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -558,7 +574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -569,25 +585,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implemented API version of get company Info flow, will look to improve background processing for the rest of demo process tomorrow - need to ask others about folder structure for running this flow
</commit_message>
<xml_diff>
--- a/demoRobot/Documents/Config/config.xlsx
+++ b/demoRobot/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\dracoe\demoRobot\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC77B70-11D2-47ED-AC5D-33B9F1372F74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0EE48B-A389-40B8-BBD8-2340AA6555CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve"> ROBOT PARAMETERS</t>
   </si>
   <si>
-    <t>Regex</t>
-  </si>
-  <si>
     <t>boolBreakpoint1</t>
   </si>
   <si>
@@ -88,6 +85,15 @@
   </si>
   <si>
     <t>The title of the start pop up.</t>
+  </si>
+  <si>
+    <t>The file path for storing email attachments</t>
+  </si>
+  <si>
+    <t>AttachmentDirectory</t>
+  </si>
+  <si>
+    <t>{0}\Desktop\Attachments</t>
   </si>
 </sst>
 </file>
@@ -213,7 +219,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C10" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -520,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,13 +542,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -554,78 +560,87 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>1</v>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
demo robot in reframework progress and OCRDeepDive project added
</commit_message>
<xml_diff>
--- a/demoRobot/Documents/Config/config.xlsx
+++ b/demoRobot/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\dracoe\demoRobot\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0EE48B-A389-40B8-BBD8-2340AA6555CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5B98E2-EAFA-4BC7-AC05-E17761CCCFBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve"> ROBOT PARAMETERS</t>
   </si>
@@ -42,9 +42,6 @@
     <t>outlook email account</t>
   </si>
   <si>
-    <t>Sean.Crotty@defra.gov.uk</t>
-  </si>
-  <si>
     <t>LogFilePath</t>
   </si>
   <si>
@@ -72,12 +69,6 @@
     <t>workpackage name</t>
   </si>
   <si>
-    <t>StartPopUpText</t>
-  </si>
-  <si>
-    <t>The popup text to be displayed to the user at the start of the process.</t>
-  </si>
-  <si>
     <t>StartPopUpTitle</t>
   </si>
   <si>
@@ -94,6 +85,63 @@
   </si>
   <si>
     <t>{0}\Desktop\Attachments</t>
+  </si>
+  <si>
+    <t>Jason.Savory@defra.gov.uk</t>
+  </si>
+  <si>
+    <t>The folder to look for the mail for processing</t>
+  </si>
+  <si>
+    <t>Email to process folder</t>
+  </si>
+  <si>
+    <t>Email in progress folder</t>
+  </si>
+  <si>
+    <t>The folder to move for in progress</t>
+  </si>
+  <si>
+    <t>Email complete folder</t>
+  </si>
+  <si>
+    <t>The folder to move for completed mail</t>
+  </si>
+  <si>
+    <t>Email exception folder</t>
+  </si>
+  <si>
+    <t>The folder to move exceptioned mail</t>
+  </si>
+  <si>
+    <t>Inbox\COMPANY INFO\For Processing</t>
+  </si>
+  <si>
+    <t>Inbox\COMPANY INFO\In Progress</t>
+  </si>
+  <si>
+    <t>Inbox\COMPANY INFO\Completed</t>
+  </si>
+  <si>
+    <t>Inbox\COMPANY INFO\Exceptions</t>
+  </si>
+  <si>
+    <t>RunTypeAssetName</t>
+  </si>
+  <si>
+    <t>The asset name to control attended/unattended run</t>
+  </si>
+  <si>
+    <t>DEMO_RUN_TYPE</t>
+  </si>
+  <si>
+    <t>Orchestrator Folder Path</t>
+  </si>
+  <si>
+    <t>The path to the orcehstrator folder containing this process</t>
+  </si>
+  <si>
+    <t>EA Root/Utilities</t>
   </si>
 </sst>
 </file>
@@ -219,7 +267,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C14" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -526,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,13 +590,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -571,13 +619,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -585,7 +633,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>4</v>
@@ -593,54 +641,102 @@
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>